<commit_message>
update: changing the master-spreadsheet funding sheet to match with button functionality
</commit_message>
<xml_diff>
--- a/master_spreadsheet_summer_25_26.xlsx
+++ b/master_spreadsheet_summer_25_26.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Intern\WEHI\prod\forecasting-with-workday-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F5AF94-8504-4E2B-8299-A6698D557DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110D7186-7B96-4100-91D7-04400D60CD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Funding" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
   <si>
     <t>Source ID</t>
   </si>
@@ -155,6 +155,18 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Cancer Research Grant</t>
+  </si>
+  <si>
+    <t>Clinical Trial Funding</t>
+  </si>
+  <si>
+    <t>Internal Research Fund</t>
+  </si>
+  <si>
+    <t>Funding Source</t>
   </si>
 </sst>
 </file>
@@ -219,33 +231,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,216 +535,250 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="43.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="28.8">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="11"/>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:7" ht="43.2">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4">
+      <c r="D2" s="4">
         <v>45658</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>45838</v>
       </c>
-      <c r="E2" s="5">
+      <c r="F2" s="5">
         <v>15000</v>
       </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" ht="28.8">
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4">
+      <c r="D3" s="4">
         <v>45689</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>45900</v>
       </c>
-      <c r="E3" s="5">
+      <c r="F3" s="5">
         <v>12000</v>
       </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="43.2">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4">
+      <c r="D4" s="4">
         <v>45717</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <v>45930</v>
       </c>
-      <c r="E4" s="5">
+      <c r="F4" s="5">
         <v>8000</v>
       </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="28.8">
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="43.2">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="4">
+      <c r="D5" s="4">
         <v>45658</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="4">
         <v>46022</v>
       </c>
-      <c r="E5" s="5">
+      <c r="F5" s="5">
         <v>20000</v>
       </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" ht="28.8">
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" ht="43.2">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="4">
+      <c r="D6" s="4">
         <v>45748</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E6" s="4">
         <v>45961</v>
       </c>
-      <c r="E6" s="5">
+      <c r="F6" s="5">
         <v>10000</v>
       </c>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" ht="43.2">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4">
+      <c r="D7" s="4">
         <v>45809</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E7" s="4">
         <v>46022</v>
       </c>
-      <c r="E7" s="5">
+      <c r="F7" s="5">
         <v>18000</v>
       </c>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" ht="28.8">
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="43.2">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="4">
+      <c r="D8" s="4">
         <v>45658</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="4">
         <v>46022</v>
       </c>
-      <c r="E8" s="5">
+      <c r="F8" s="5">
         <v>25000</v>
       </c>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" ht="43.2">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="4">
+      <c r="D9" s="4">
         <v>45778</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E9" s="4">
         <v>45991</v>
       </c>
-      <c r="E9" s="5">
+      <c r="F9" s="5">
         <v>5000</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="43.2">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="4">
+      <c r="D10" s="4">
         <v>45839</v>
       </c>
-      <c r="D10" s="4">
+      <c r="E10" s="4">
         <v>46022</v>
       </c>
-      <c r="E10" s="5">
+      <c r="F10" s="5">
         <v>14000</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" ht="43.2">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="4">
+      <c r="D11" s="4">
         <v>45658</v>
       </c>
-      <c r="D11" s="4">
+      <c r="E11" s="4">
         <v>46022</v>
       </c>
-      <c r="E11" s="5">
+      <c r="F11" s="5">
         <v>10000</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1"/>
@@ -746,6 +787,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1"/>
@@ -754,6 +796,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1"/>
@@ -762,6 +805,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1"/>
@@ -770,6 +814,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1"/>
@@ -778,6 +823,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -802,22 +848,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="43.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>